<commit_message>
Update log and pillow version
</commit_message>
<xml_diff>
--- a/Examples/test_data/BasicNonTestResultColumnsMultipleSheet.xlsx
+++ b/Examples/test_data/BasicNonTestResultColumnsMultipleSheet.xlsx
@@ -1,97 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\atthaboon\Documents\GitHub\robotframework-ExcelDataDriver\Examples\test_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F59E87-DB19-47DD-84D5-2F4AE1D1D51E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="165" windowWidth="16305" windowHeight="10245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4035" yWindow="165" windowWidth="16305" windowHeight="10245" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="missing all" sheetId="1" r:id="rId1"/>
-    <sheet name="row 2 and some column" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="missing all" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="row 2 and some column" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
-  <si>
-    <t>[Tags]</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>demo1</t>
-  </si>
-  <si>
-    <t>Welcome1</t>
-  </si>
-  <si>
-    <t>demo@demo.com</t>
-  </si>
-  <si>
-    <t>demo2</t>
-  </si>
-  <si>
-    <t>demo</t>
-  </si>
-  <si>
-    <t>demo3</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,25 +85,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -443,55 +394,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>[Status]</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>[Log Message]</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>[Screenshot]</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>[Tags]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>demo1</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Welcome1</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>demo@demo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>demo2</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Welcome1</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>demo3</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>demo@demo.com</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -501,61 +498,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col width="17.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>[Status]</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[Log Message]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[Screenshot]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[Tags]</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>demo1</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Welcome1</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>demo@demo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>demo2</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Welcome1</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>demo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>demo3</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>demo@demo.com</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>